<commit_message>
New UniProt downlad for Humans.
</commit_message>
<xml_diff>
--- a/biodownloads/quora/chrY_proteins.xlsx
+++ b/biodownloads/quora/chrY_proteins.xlsx
@@ -19,10 +19,10 @@
     <t>Human Chromosome Y: 239 proteins from 65 out of 74 NCBI protein-coding genes</t>
   </si>
   <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Symbol</t>
+    <t>Protein AC</t>
+  </si>
+  <si>
+    <t>Gene</t>
   </si>
   <si>
     <t>Recommended Protein Name</t>

</xml_diff>